<commit_message>
Added more characters to Pixelfont
</commit_message>
<xml_diff>
--- a/sources/PixelFont.xlsx
+++ b/sources/PixelFont.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewgraham/Development/Fonts/excel-font/sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{253F17A7-4B2A-3148-B55B-920B9AAD2BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925C2FBC-D9E4-9D48-9FE9-868580666FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="30360" windowHeight="17260" xr2:uid="{2336CB7C-6D9B-7C47-9140-73EF9BB26195}"/>
+    <workbookView xWindow="9700" yWindow="500" windowWidth="26080" windowHeight="17820" xr2:uid="{2336CB7C-6D9B-7C47-9140-73EF9BB26195}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="64">
   <si>
     <t>A</t>
   </si>
@@ -102,6 +102,9 @@
     <t>L</t>
   </si>
   <si>
+    <t>m</t>
+  </si>
+  <si>
     <t>M</t>
   </si>
   <si>
@@ -123,6 +126,9 @@
     <t>S</t>
   </si>
   <si>
+    <t>s</t>
+  </si>
+  <si>
     <t>T</t>
   </si>
   <si>
@@ -154,6 +160,72 @@
   </si>
   <si>
     <t>bottom</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>space</t>
+  </si>
+  <si>
+    <t>period</t>
+  </si>
+  <si>
+    <t>comma</t>
+  </si>
+  <si>
+    <t>quotesingle</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
   </si>
 </sst>
 </file>
@@ -196,7 +268,42 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -528,15 +635,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F65F842-B661-8A42-8744-5CD5F407DFB4}">
-  <dimension ref="A1:BU42"/>
+  <dimension ref="A1:BU84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="AJ30" sqref="AJ30"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="AE77" sqref="AE77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.83203125" customWidth="1"/>
+    <col min="2" max="72" width="2.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:73" x14ac:dyDescent="0.2">
@@ -762,7 +870,7 @@
     </row>
     <row r="2" spans="1:73" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:73" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1331,7 +1439,7 @@
     </row>
     <row r="14" spans="1:73" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:73" x14ac:dyDescent="0.2">
@@ -1357,189 +1465,189 @@
         <v>21</v>
       </c>
       <c r="H15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Q15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="R15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="V15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="W15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="X15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Y15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Z15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AA15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AB15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AC15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AD15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AE15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AF15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AG15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AH15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AI15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AJ15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AK15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AL15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AM15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AN15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AO15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AP15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AQ15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AR15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AS15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AT15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AU15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AV15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AW15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AX15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AY15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AZ15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="BA15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="BB15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="BC15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="BD15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="BE15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="BF15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="BG15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="BH15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="BI15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="BJ15" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="BK15" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="BL15" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="BM15" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="BN15" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:73" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
@@ -1619,7 +1727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C18" s="1">
         <v>1</v>
       </c>
@@ -1678,7 +1786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -1737,7 +1845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C20" s="1">
         <v>1</v>
       </c>
@@ -1805,7 +1913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C21" s="1">
         <v>1</v>
       </c>
@@ -1852,7 +1960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C22" s="1">
         <v>1</v>
       </c>
@@ -1902,7 +2010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C23" s="1">
         <v>1</v>
       </c>
@@ -1952,7 +2060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C24" s="1">
         <v>1</v>
       </c>
@@ -2017,291 +2125,306 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:70" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="C29" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="D29" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="E29" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="F29" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="G29" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="H29" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="I29" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="J29" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="K29" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="L29" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="M29" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="N29" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="O29" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="P29" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="Q29" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="R29" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="S29" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="T29" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="U29" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="V29" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="W29" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="X29" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="Y29" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="Z29" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="AA29" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="AB29" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="AC29" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="AD29" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="AE29" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="AF29" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="AG29" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="AH29" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="AI29" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="AJ29" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="AK29" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="AL29" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="AM29" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="AN29" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="AO29" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="AP29" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="AQ29" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="AR29" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="AS29" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="AT29" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="AU29" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="AV29" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="AW29" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="AX29" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="AY29" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="AZ29" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="BA29" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="BB29" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="BC29" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="BD29" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="BE29" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="BF29" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="BG29" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="BH29" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="BI29" t="s">
-        <v>19</v>
-      </c>
-      <c r="BJ29" t="s">
-        <v>36</v>
-      </c>
-      <c r="BK29" t="s">
-        <v>36</v>
-      </c>
-      <c r="BL29" t="s">
-        <v>36</v>
-      </c>
-      <c r="BM29" t="s">
-        <v>36</v>
-      </c>
-      <c r="BN29" t="s">
-        <v>36</v>
-      </c>
-      <c r="BO29" t="s">
-        <v>36</v>
-      </c>
-      <c r="BP29" t="s">
-        <v>37</v>
-      </c>
-      <c r="BQ29" t="s">
-        <v>37</v>
-      </c>
-      <c r="BR29" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1</v>
+      </c>
       <c r="J31" s="1">
         <v>1</v>
       </c>
-      <c r="AA31" s="1">
-        <v>1</v>
-      </c>
-      <c r="AK31" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AL31" s="1">
-        <v>1</v>
-      </c>
-      <c r="AM31" s="1">
-        <v>1</v>
-      </c>
-      <c r="AW31" s="1">
-        <v>1</v>
-      </c>
-      <c r="BD31" s="1">
+      <c r="N31" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>1</v>
+      </c>
+      <c r="W31" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z31" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD31" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG31" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK31" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN31" s="1">
+        <v>1</v>
+      </c>
+      <c r="AO31" s="1">
+        <v>1</v>
+      </c>
+      <c r="AP31" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ31" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR31" s="1">
+        <v>1</v>
+      </c>
+      <c r="BG31" s="1">
         <v>1</v>
       </c>
       <c r="BH31" s="1">
         <v>1</v>
       </c>
-      <c r="BK31" s="1">
-        <v>1</v>
-      </c>
-      <c r="BQ31" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="G32" s="1">
+        <v>1</v>
+      </c>
       <c r="J32" s="1">
         <v>1</v>
       </c>
-      <c r="AA32" s="1">
+      <c r="N32" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>1</v>
+      </c>
+      <c r="W32" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z32" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD32" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG32" s="1">
         <v>1</v>
       </c>
       <c r="AK32" s="1">
         <v>1</v>
       </c>
-      <c r="AW32" s="1">
-        <v>1</v>
-      </c>
-      <c r="BK32" s="1">
-        <v>1</v>
-      </c>
-      <c r="BQ32" s="1">
+      <c r="AR32" s="1">
+        <v>1</v>
+      </c>
+      <c r="BG32" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH32" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2309,179 +2432,80 @@
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D33" s="1">
-        <v>1</v>
-      </c>
-      <c r="E33" s="1">
-        <v>1</v>
-      </c>
-      <c r="F33" s="1">
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="G33" s="1">
         <v>1</v>
       </c>
       <c r="J33" s="1">
         <v>1</v>
       </c>
-      <c r="L33" s="1">
-        <v>1</v>
-      </c>
-      <c r="M33" s="1">
-        <v>1</v>
-      </c>
-      <c r="R33" s="1">
-        <v>1</v>
-      </c>
-      <c r="S33" s="1">
-        <v>1</v>
-      </c>
-      <c r="T33" s="1">
-        <v>1</v>
-      </c>
-      <c r="X33" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y33" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z33" s="1">
+      <c r="N33" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>1</v>
+      </c>
+      <c r="W33" s="1">
         <v>1</v>
       </c>
       <c r="AA33" s="1">
         <v>1</v>
       </c>
-      <c r="AE33" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF33" s="1">
+      <c r="AC33" s="1">
         <v>1</v>
       </c>
       <c r="AG33" s="1">
         <v>1</v>
       </c>
-      <c r="AJ33" s="1">
-        <v>1</v>
-      </c>
       <c r="AK33" s="1">
         <v>1</v>
       </c>
-      <c r="AL33" s="1">
-        <v>1</v>
-      </c>
-      <c r="AM33" s="1">
-        <v>1</v>
-      </c>
       <c r="AQ33" s="1">
         <v>1</v>
       </c>
-      <c r="AR33" s="1">
-        <v>1</v>
-      </c>
-      <c r="AS33" s="1">
-        <v>1</v>
-      </c>
-      <c r="AT33" s="1">
-        <v>1</v>
-      </c>
-      <c r="AW33" s="1">
-        <v>1</v>
-      </c>
-      <c r="AY33" s="1">
-        <v>1</v>
-      </c>
-      <c r="AZ33" s="1">
-        <v>1</v>
-      </c>
-      <c r="BD33" s="1">
-        <v>1</v>
-      </c>
       <c r="BH33" s="1">
         <v>1</v>
       </c>
-      <c r="BK33" s="1">
-        <v>1</v>
-      </c>
-      <c r="BN33" s="1">
-        <v>1</v>
-      </c>
-      <c r="BQ33" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="34" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
       <c r="G34" s="1">
         <v>1</v>
       </c>
       <c r="J34" s="1">
         <v>1</v>
       </c>
-      <c r="K34" s="1">
-        <v>1</v>
-      </c>
       <c r="N34" s="1">
         <v>1</v>
       </c>
       <c r="Q34" s="1">
         <v>1</v>
       </c>
-      <c r="T34" s="1">
-        <v>1</v>
-      </c>
       <c r="W34" s="1">
         <v>1</v>
       </c>
-      <c r="AA34" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD34" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG34" s="1">
-        <v>1</v>
-      </c>
-      <c r="AK34" s="1">
+      <c r="AB34" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH34" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ34" s="1">
         <v>1</v>
       </c>
       <c r="AP34" s="1">
         <v>1</v>
       </c>
-      <c r="AS34" s="1">
-        <v>1</v>
-      </c>
-      <c r="AW34" s="1">
-        <v>1</v>
-      </c>
-      <c r="AX34" s="1">
-        <v>1</v>
-      </c>
-      <c r="BA34" s="1">
-        <v>1</v>
-      </c>
-      <c r="BD34" s="1">
-        <v>1</v>
-      </c>
-      <c r="BH34" s="1">
-        <v>1</v>
-      </c>
-      <c r="BK34" s="1">
-        <v>1</v>
-      </c>
-      <c r="BM34" s="1">
-        <v>1</v>
-      </c>
-      <c r="BQ34" s="1">
+      <c r="BG34" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C35" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="1">
-        <v>1</v>
-      </c>
-      <c r="E35" s="1">
-        <v>1</v>
-      </c>
-      <c r="F35" s="1">
+      <c r="C35" s="1">
         <v>1</v>
       </c>
       <c r="G35" s="1">
@@ -2496,46 +2520,22 @@
       <c r="Q35" s="1">
         <v>1</v>
       </c>
+      <c r="T35" s="1">
+        <v>1</v>
+      </c>
       <c r="W35" s="1">
         <v>1</v>
       </c>
       <c r="AA35" s="1">
         <v>1</v>
       </c>
-      <c r="AD35" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF35" s="1">
-        <v>1</v>
-      </c>
-      <c r="AK35" s="1">
+      <c r="AC35" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI35" s="1">
         <v>1</v>
       </c>
       <c r="AP35" s="1">
-        <v>1</v>
-      </c>
-      <c r="AS35" s="1">
-        <v>1</v>
-      </c>
-      <c r="AW35" s="1">
-        <v>1</v>
-      </c>
-      <c r="BA35" s="1">
-        <v>1</v>
-      </c>
-      <c r="BD35" s="1">
-        <v>1</v>
-      </c>
-      <c r="BH35" s="1">
-        <v>1</v>
-      </c>
-      <c r="BK35" s="1">
-        <v>1</v>
-      </c>
-      <c r="BL35" s="1">
-        <v>1</v>
-      </c>
-      <c r="BQ35" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2546,55 +2546,31 @@
       <c r="G36" s="1">
         <v>1</v>
       </c>
-      <c r="J36" s="1">
-        <v>1</v>
-      </c>
-      <c r="N36" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q36" s="1">
-        <v>1</v>
-      </c>
-      <c r="W36" s="1">
+      <c r="K36" s="1">
+        <v>1</v>
+      </c>
+      <c r="M36" s="1">
+        <v>1</v>
+      </c>
+      <c r="R36" s="1">
+        <v>1</v>
+      </c>
+      <c r="T36" s="1">
+        <v>1</v>
+      </c>
+      <c r="V36" s="1">
         <v>1</v>
       </c>
       <c r="AA36" s="1">
         <v>1</v>
       </c>
-      <c r="AD36" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE36" s="1">
-        <v>1</v>
-      </c>
-      <c r="AK36" s="1">
-        <v>1</v>
-      </c>
-      <c r="AQ36" s="1">
-        <v>1</v>
-      </c>
-      <c r="AR36" s="1">
-        <v>1</v>
-      </c>
-      <c r="AW36" s="1">
-        <v>1</v>
-      </c>
-      <c r="BA36" s="1">
-        <v>1</v>
-      </c>
-      <c r="BD36" s="1">
-        <v>1</v>
-      </c>
-      <c r="BH36" s="1">
-        <v>1</v>
-      </c>
-      <c r="BK36" s="1">
-        <v>1</v>
-      </c>
-      <c r="BM36" s="1">
-        <v>1</v>
-      </c>
-      <c r="BQ36" s="1">
+      <c r="AC36" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI36" s="1">
+        <v>1</v>
+      </c>
+      <c r="AO36" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2602,58 +2578,46 @@
       <c r="C37" s="1">
         <v>1</v>
       </c>
-      <c r="F37" s="1">
-        <v>1</v>
-      </c>
       <c r="G37" s="1">
         <v>1</v>
       </c>
-      <c r="J37" s="1">
-        <v>1</v>
-      </c>
-      <c r="N37" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q37" s="1">
-        <v>1</v>
-      </c>
-      <c r="W37" s="1">
+      <c r="K37" s="1">
+        <v>1</v>
+      </c>
+      <c r="M37" s="1">
+        <v>1</v>
+      </c>
+      <c r="R37" s="1">
+        <v>1</v>
+      </c>
+      <c r="T37" s="1">
+        <v>1</v>
+      </c>
+      <c r="V37" s="1">
         <v>1</v>
       </c>
       <c r="Z37" s="1">
         <v>1</v>
       </c>
-      <c r="AA37" s="1">
-        <v>1</v>
-      </c>
       <c r="AD37" s="1">
         <v>1</v>
       </c>
-      <c r="AK37" s="1">
-        <v>1</v>
-      </c>
-      <c r="AP37" s="1">
-        <v>1</v>
-      </c>
-      <c r="AW37" s="1">
-        <v>1</v>
-      </c>
-      <c r="BA37" s="1">
+      <c r="AI37" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN37" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY37" s="1">
+        <v>1</v>
+      </c>
+      <c r="AZ37" s="1">
+        <v>1</v>
+      </c>
+      <c r="BC37" s="1">
         <v>1</v>
       </c>
       <c r="BD37" s="1">
-        <v>1</v>
-      </c>
-      <c r="BH37" s="1">
-        <v>1</v>
-      </c>
-      <c r="BK37" s="1">
-        <v>1</v>
-      </c>
-      <c r="BN37" s="1">
-        <v>1</v>
-      </c>
-      <c r="BQ37" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2664,52 +2628,31 @@
       <c r="E38" s="1">
         <v>1</v>
       </c>
-      <c r="G38" s="1">
-        <v>1</v>
-      </c>
-      <c r="H38" s="1">
-        <v>1</v>
-      </c>
-      <c r="J38" s="1">
-        <v>1</v>
-      </c>
-      <c r="K38" s="1">
+      <c r="F38" s="1">
         <v>1</v>
       </c>
       <c r="L38" s="1">
         <v>1</v>
       </c>
-      <c r="M38" s="1">
-        <v>1</v>
-      </c>
-      <c r="R38" s="1">
-        <v>1</v>
-      </c>
       <c r="S38" s="1">
         <v>1</v>
       </c>
-      <c r="T38" s="1">
-        <v>1</v>
-      </c>
-      <c r="X38" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y38" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA38" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE38" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF38" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG38" s="1">
-        <v>1</v>
-      </c>
-      <c r="AK38" s="1">
+      <c r="U38" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z38" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD38" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI38" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN38" s="1">
+        <v>1</v>
+      </c>
+      <c r="AO38" s="1">
         <v>1</v>
       </c>
       <c r="AP38" s="1">
@@ -2721,28 +2664,16 @@
       <c r="AR38" s="1">
         <v>1</v>
       </c>
-      <c r="AS38" s="1">
-        <v>1</v>
-      </c>
-      <c r="AW38" s="1">
-        <v>1</v>
-      </c>
-      <c r="BA38" s="1">
-        <v>1</v>
-      </c>
-      <c r="BE38" s="1">
-        <v>1</v>
-      </c>
-      <c r="BH38" s="1">
-        <v>1</v>
-      </c>
-      <c r="BK38" s="1">
-        <v>1</v>
-      </c>
-      <c r="BO38" s="1">
-        <v>1</v>
-      </c>
-      <c r="BR38" s="1">
+      <c r="AY38" s="1">
+        <v>1</v>
+      </c>
+      <c r="AZ38" s="1">
+        <v>1</v>
+      </c>
+      <c r="BC38" s="1">
+        <v>1</v>
+      </c>
+      <c r="BD38" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2750,30 +2681,15 @@
       <c r="A39" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AT39" s="1">
-        <v>1</v>
-      </c>
-      <c r="BH39" s="1">
+      <c r="BD39" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="AP40" s="1">
-        <v>1</v>
-      </c>
-      <c r="AQ40" s="1">
-        <v>1</v>
-      </c>
-      <c r="AR40" s="1">
-        <v>1</v>
-      </c>
-      <c r="AS40" s="1">
-        <v>1</v>
-      </c>
       <c r="AT40" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="BG40" s="1">
+      <c r="BC40" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2784,21 +2700,2008 @@
     </row>
     <row r="42" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" t="s">
+        <v>3</v>
+      </c>
+      <c r="F43" t="s">
+        <v>3</v>
+      </c>
+      <c r="G43" t="s">
+        <v>3</v>
+      </c>
+      <c r="H43" t="s">
+        <v>3</v>
+      </c>
+      <c r="I43" t="s">
+        <v>4</v>
+      </c>
+      <c r="J43" t="s">
+        <v>4</v>
+      </c>
+      <c r="K43" t="s">
+        <v>4</v>
+      </c>
+      <c r="L43" t="s">
+        <v>4</v>
+      </c>
+      <c r="M43" t="s">
+        <v>4</v>
+      </c>
+      <c r="N43" t="s">
+        <v>4</v>
+      </c>
+      <c r="O43" t="s">
+        <v>4</v>
+      </c>
+      <c r="P43" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>5</v>
+      </c>
+      <c r="R43" t="s">
+        <v>5</v>
+      </c>
+      <c r="S43" t="s">
+        <v>5</v>
+      </c>
+      <c r="T43" t="s">
+        <v>5</v>
+      </c>
+      <c r="U43" t="s">
+        <v>5</v>
+      </c>
+      <c r="V43" t="s">
+        <v>32</v>
+      </c>
+      <c r="W43" t="s">
+        <v>32</v>
+      </c>
+      <c r="X43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z43" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA43" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC43" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD43" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE43" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF43" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG43" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH43" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI43" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ43" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK43" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL43" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM43" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN43" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO43" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP43" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ43" t="s">
+        <v>35</v>
+      </c>
+      <c r="AR43" t="s">
+        <v>35</v>
+      </c>
+      <c r="AS43" t="s">
+        <v>35</v>
+      </c>
+      <c r="AT43" t="s">
+        <v>35</v>
+      </c>
+      <c r="AU43" t="s">
+        <v>35</v>
+      </c>
+      <c r="AV43" t="s">
+        <v>36</v>
+      </c>
+      <c r="AW43" t="s">
+        <v>36</v>
+      </c>
+      <c r="AX43" t="s">
+        <v>36</v>
+      </c>
+      <c r="AY43" t="s">
+        <v>36</v>
+      </c>
+      <c r="AZ43" t="s">
+        <v>36</v>
+      </c>
+      <c r="BA43" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB43" t="s">
+        <v>36</v>
+      </c>
+      <c r="BC43" t="s">
+        <v>37</v>
+      </c>
+      <c r="BD43" t="s">
+        <v>37</v>
+      </c>
+      <c r="BE43" t="s">
+        <v>37</v>
+      </c>
+      <c r="BF43" t="s">
+        <v>19</v>
+      </c>
+      <c r="BG43" t="s">
+        <v>19</v>
+      </c>
+      <c r="BH43" t="s">
+        <v>19</v>
+      </c>
+      <c r="BI43" t="s">
+        <v>19</v>
+      </c>
+      <c r="BJ43" t="s">
+        <v>38</v>
+      </c>
+      <c r="BK43" t="s">
+        <v>38</v>
+      </c>
+      <c r="BL43" t="s">
+        <v>38</v>
+      </c>
+      <c r="BM43" t="s">
+        <v>38</v>
+      </c>
+      <c r="BN43" t="s">
+        <v>38</v>
+      </c>
+      <c r="BO43" t="s">
+        <v>38</v>
+      </c>
+      <c r="BP43" t="s">
         <v>39</v>
       </c>
+      <c r="BQ43" t="s">
+        <v>39</v>
+      </c>
+      <c r="BR43" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW45" s="1">
+        <v>1</v>
+      </c>
+      <c r="BD45" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH45" s="1">
+        <v>1</v>
+      </c>
+      <c r="BK45" s="1">
+        <v>1</v>
+      </c>
+      <c r="BQ45" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J46" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA46" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK46" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW46" s="1">
+        <v>1</v>
+      </c>
+      <c r="BK46" s="1">
+        <v>1</v>
+      </c>
+      <c r="BQ46" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1</v>
+      </c>
+      <c r="E47" s="1">
+        <v>1</v>
+      </c>
+      <c r="F47" s="1">
+        <v>1</v>
+      </c>
+      <c r="J47" s="1">
+        <v>1</v>
+      </c>
+      <c r="L47" s="1">
+        <v>1</v>
+      </c>
+      <c r="M47" s="1">
+        <v>1</v>
+      </c>
+      <c r="R47" s="1">
+        <v>1</v>
+      </c>
+      <c r="S47" s="1">
+        <v>1</v>
+      </c>
+      <c r="T47" s="1">
+        <v>1</v>
+      </c>
+      <c r="X47" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y47" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AT47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AZ47" s="1">
+        <v>1</v>
+      </c>
+      <c r="BD47" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH47" s="1">
+        <v>1</v>
+      </c>
+      <c r="BK47" s="1">
+        <v>1</v>
+      </c>
+      <c r="BN47" s="1">
+        <v>1</v>
+      </c>
+      <c r="BQ47" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G48" s="1">
+        <v>1</v>
+      </c>
+      <c r="J48" s="1">
+        <v>1</v>
+      </c>
+      <c r="K48" s="1">
+        <v>1</v>
+      </c>
+      <c r="N48" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q48" s="1">
+        <v>1</v>
+      </c>
+      <c r="T48" s="1">
+        <v>1</v>
+      </c>
+      <c r="W48" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA48" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD48" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG48" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK48" s="1">
+        <v>1</v>
+      </c>
+      <c r="AP48" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS48" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW48" s="1">
+        <v>1</v>
+      </c>
+      <c r="AX48" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA48" s="1">
+        <v>1</v>
+      </c>
+      <c r="BD48" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH48" s="1">
+        <v>1</v>
+      </c>
+      <c r="BK48" s="1">
+        <v>1</v>
+      </c>
+      <c r="BM48" s="1">
+        <v>1</v>
+      </c>
+      <c r="BQ48" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C49" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1</v>
+      </c>
+      <c r="E49" s="1">
+        <v>1</v>
+      </c>
+      <c r="F49" s="1">
+        <v>1</v>
+      </c>
+      <c r="G49" s="1">
+        <v>1</v>
+      </c>
+      <c r="J49" s="1">
+        <v>1</v>
+      </c>
+      <c r="N49" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q49" s="1">
+        <v>1</v>
+      </c>
+      <c r="W49" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA49" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD49" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF49" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK49" s="1">
+        <v>1</v>
+      </c>
+      <c r="AP49" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS49" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW49" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA49" s="1">
+        <v>1</v>
+      </c>
+      <c r="BD49" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH49" s="1">
+        <v>1</v>
+      </c>
+      <c r="BK49" s="1">
+        <v>1</v>
+      </c>
+      <c r="BL49" s="1">
+        <v>1</v>
+      </c>
+      <c r="BQ49" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C50" s="1">
+        <v>1</v>
+      </c>
+      <c r="G50" s="1">
+        <v>1</v>
+      </c>
+      <c r="J50" s="1">
+        <v>1</v>
+      </c>
+      <c r="N50" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q50" s="1">
+        <v>1</v>
+      </c>
+      <c r="W50" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA50" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD50" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE50" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK50" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ50" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR50" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW50" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA50" s="1">
+        <v>1</v>
+      </c>
+      <c r="BD50" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH50" s="1">
+        <v>1</v>
+      </c>
+      <c r="BK50" s="1">
+        <v>1</v>
+      </c>
+      <c r="BM50" s="1">
+        <v>1</v>
+      </c>
+      <c r="BQ50" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C51" s="1">
+        <v>1</v>
+      </c>
+      <c r="F51" s="1">
+        <v>1</v>
+      </c>
+      <c r="G51" s="1">
+        <v>1</v>
+      </c>
+      <c r="J51" s="1">
+        <v>1</v>
+      </c>
+      <c r="N51" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q51" s="1">
+        <v>1</v>
+      </c>
+      <c r="W51" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z51" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA51" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD51" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK51" s="1">
+        <v>1</v>
+      </c>
+      <c r="AP51" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW51" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA51" s="1">
+        <v>1</v>
+      </c>
+      <c r="BD51" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH51" s="1">
+        <v>1</v>
+      </c>
+      <c r="BK51" s="1">
+        <v>1</v>
+      </c>
+      <c r="BN51" s="1">
+        <v>1</v>
+      </c>
+      <c r="BQ51" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D52" s="1">
+        <v>1</v>
+      </c>
+      <c r="E52" s="1">
+        <v>1</v>
+      </c>
+      <c r="G52" s="1">
+        <v>1</v>
+      </c>
+      <c r="H52" s="1">
+        <v>1</v>
+      </c>
+      <c r="J52" s="1">
+        <v>1</v>
+      </c>
+      <c r="K52" s="1">
+        <v>1</v>
+      </c>
+      <c r="L52" s="1">
+        <v>1</v>
+      </c>
+      <c r="M52" s="1">
+        <v>1</v>
+      </c>
+      <c r="R52" s="1">
+        <v>1</v>
+      </c>
+      <c r="S52" s="1">
+        <v>1</v>
+      </c>
+      <c r="T52" s="1">
+        <v>1</v>
+      </c>
+      <c r="X52" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y52" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA52" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE52" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF52" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG52" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK52" s="1">
+        <v>1</v>
+      </c>
+      <c r="AP52" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ52" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR52" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS52" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW52" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA52" s="1">
+        <v>1</v>
+      </c>
+      <c r="BE52" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH52" s="1">
+        <v>1</v>
+      </c>
+      <c r="BK52" s="1">
+        <v>1</v>
+      </c>
+      <c r="BO52" s="1">
+        <v>1</v>
+      </c>
+      <c r="BR52" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT53" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH53" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AP54" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ54" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR54" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS54" s="1">
+        <v>1</v>
+      </c>
+      <c r="AT54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="BG54" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:70" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>11</v>
+      </c>
+      <c r="B57" t="s">
+        <v>22</v>
+      </c>
+      <c r="C57" t="s">
+        <v>22</v>
+      </c>
+      <c r="D57" t="s">
+        <v>22</v>
+      </c>
+      <c r="E57" t="s">
+        <v>22</v>
+      </c>
+      <c r="F57" t="s">
+        <v>22</v>
+      </c>
+      <c r="G57" t="s">
+        <v>22</v>
+      </c>
+      <c r="H57" t="s">
+        <v>22</v>
+      </c>
+      <c r="I57" t="s">
+        <v>22</v>
+      </c>
+      <c r="J57" t="s">
+        <v>22</v>
+      </c>
+      <c r="K57" t="s">
+        <v>52</v>
+      </c>
+      <c r="L57" t="s">
+        <v>52</v>
+      </c>
+      <c r="M57" t="s">
+        <v>52</v>
+      </c>
+      <c r="N57" t="s">
+        <v>52</v>
+      </c>
+      <c r="O57" t="s">
+        <v>52</v>
+      </c>
+      <c r="P57" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>52</v>
+      </c>
+      <c r="R57" t="s">
+        <v>53</v>
+      </c>
+      <c r="S57" t="s">
+        <v>53</v>
+      </c>
+      <c r="T57" t="s">
+        <v>53</v>
+      </c>
+      <c r="U57" t="s">
+        <v>53</v>
+      </c>
+      <c r="V57" t="s">
+        <v>53</v>
+      </c>
+      <c r="W57" t="s">
+        <v>53</v>
+      </c>
+      <c r="X57" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y57" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z57" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA57" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB57" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC57" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD57" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE57" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF57" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG57" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH57" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI57" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ57" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK57" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL57" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM57" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN57" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO57" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP57" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ57" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR57" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS57" t="s">
+        <v>30</v>
+      </c>
+      <c r="AT57" t="s">
+        <v>30</v>
+      </c>
+      <c r="AU57" t="s">
+        <v>30</v>
+      </c>
+      <c r="AV57" t="s">
+        <v>30</v>
+      </c>
+      <c r="AW57" t="s">
+        <v>30</v>
+      </c>
+      <c r="AX57" t="s">
+        <v>30</v>
+      </c>
+      <c r="AY57" t="s">
+        <v>57</v>
+      </c>
+      <c r="AZ57" t="s">
+        <v>57</v>
+      </c>
+      <c r="BA57" t="s">
+        <v>57</v>
+      </c>
+      <c r="BB57" t="s">
+        <v>57</v>
+      </c>
+      <c r="BC57" t="s">
+        <v>57</v>
+      </c>
+      <c r="BD57" t="s">
+        <v>57</v>
+      </c>
+      <c r="BE57" t="s">
+        <v>58</v>
+      </c>
+      <c r="BF57" t="s">
+        <v>58</v>
+      </c>
+      <c r="BG57" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH57" t="s">
+        <v>58</v>
+      </c>
+      <c r="BI57" t="s">
+        <v>58</v>
+      </c>
+      <c r="BJ57" t="s">
+        <v>58</v>
+      </c>
+      <c r="BK57" t="s">
+        <v>58</v>
+      </c>
+      <c r="BL57" t="s">
+        <v>59</v>
+      </c>
+      <c r="BM57" t="s">
+        <v>59</v>
+      </c>
+      <c r="BN57" t="s">
+        <v>59</v>
+      </c>
+      <c r="BO57" t="s">
+        <v>59</v>
+      </c>
+      <c r="BP57" t="s">
+        <v>59</v>
+      </c>
+      <c r="BQ57" t="s">
+        <v>59</v>
+      </c>
+      <c r="BR57" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+    </row>
+    <row r="59" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+      <c r="P59" s="1"/>
+    </row>
+    <row r="60" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+      <c r="BA60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1">
+        <v>1</v>
+      </c>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1">
+        <v>1</v>
+      </c>
+      <c r="F61" s="1">
+        <v>1</v>
+      </c>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1">
+        <v>1</v>
+      </c>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1">
+        <v>1</v>
+      </c>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1">
+        <v>1</v>
+      </c>
+      <c r="O61" s="1">
+        <v>1</v>
+      </c>
+      <c r="P61" s="1"/>
+      <c r="T61">
+        <v>1</v>
+      </c>
+      <c r="U61">
+        <v>1</v>
+      </c>
+      <c r="V61">
+        <v>1</v>
+      </c>
+      <c r="Z61">
+        <v>1</v>
+      </c>
+      <c r="AB61">
+        <v>1</v>
+      </c>
+      <c r="AC61">
+        <v>1</v>
+      </c>
+      <c r="AH61">
+        <v>1</v>
+      </c>
+      <c r="AI61">
+        <v>1</v>
+      </c>
+      <c r="AJ61">
+        <v>1</v>
+      </c>
+      <c r="AK61">
+        <v>1</v>
+      </c>
+      <c r="AN61">
+        <v>1</v>
+      </c>
+      <c r="AP61">
+        <v>1</v>
+      </c>
+      <c r="AQ61">
+        <v>1</v>
+      </c>
+      <c r="AU61">
+        <v>1</v>
+      </c>
+      <c r="AV61">
+        <v>1</v>
+      </c>
+      <c r="AW61">
+        <v>1</v>
+      </c>
+      <c r="AZ61">
+        <v>1</v>
+      </c>
+      <c r="BA61">
+        <v>1</v>
+      </c>
+      <c r="BB61">
+        <v>1</v>
+      </c>
+      <c r="BC61">
+        <v>1</v>
+      </c>
+      <c r="BF61">
+        <v>1</v>
+      </c>
+      <c r="BJ61">
+        <v>1</v>
+      </c>
+      <c r="BM61">
+        <v>1</v>
+      </c>
+      <c r="BQ61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1">
+        <v>1</v>
+      </c>
+      <c r="D62" s="1">
+        <v>1</v>
+      </c>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1">
+        <v>1</v>
+      </c>
+      <c r="G62" s="1">
+        <v>1</v>
+      </c>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1">
+        <v>1</v>
+      </c>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1">
+        <v>1</v>
+      </c>
+      <c r="M62" s="1">
+        <v>1</v>
+      </c>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
+      <c r="P62" s="1">
+        <v>1</v>
+      </c>
+      <c r="S62">
+        <v>1</v>
+      </c>
+      <c r="W62">
+        <v>1</v>
+      </c>
+      <c r="Z62">
+        <v>1</v>
+      </c>
+      <c r="AA62">
+        <v>1</v>
+      </c>
+      <c r="AD62">
+        <v>1</v>
+      </c>
+      <c r="AG62">
+        <v>1</v>
+      </c>
+      <c r="AK62">
+        <v>1</v>
+      </c>
+      <c r="AN62">
+        <v>1</v>
+      </c>
+      <c r="AO62">
+        <v>1</v>
+      </c>
+      <c r="AT62">
+        <v>1</v>
+      </c>
+      <c r="BA62">
+        <v>1</v>
+      </c>
+      <c r="BF62">
+        <v>1</v>
+      </c>
+      <c r="BJ62">
+        <v>1</v>
+      </c>
+      <c r="BM62">
+        <v>1</v>
+      </c>
+      <c r="BQ62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1">
+        <v>1</v>
+      </c>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1">
+        <v>1</v>
+      </c>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1">
+        <v>1</v>
+      </c>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1">
+        <v>1</v>
+      </c>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+      <c r="O63" s="1"/>
+      <c r="P63" s="1">
+        <v>1</v>
+      </c>
+      <c r="S63">
+        <v>1</v>
+      </c>
+      <c r="W63">
+        <v>1</v>
+      </c>
+      <c r="Z63">
+        <v>1</v>
+      </c>
+      <c r="AD63">
+        <v>1</v>
+      </c>
+      <c r="AG63">
+        <v>1</v>
+      </c>
+      <c r="AK63">
+        <v>1</v>
+      </c>
+      <c r="AN63">
+        <v>1</v>
+      </c>
+      <c r="AU63">
+        <v>1</v>
+      </c>
+      <c r="AV63">
+        <v>1</v>
+      </c>
+      <c r="BA63">
+        <v>1</v>
+      </c>
+      <c r="BF63">
+        <v>1</v>
+      </c>
+      <c r="BJ63">
+        <v>1</v>
+      </c>
+      <c r="BM63">
+        <v>1</v>
+      </c>
+      <c r="BQ63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1">
+        <v>1</v>
+      </c>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1">
+        <v>1</v>
+      </c>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1">
+        <v>1</v>
+      </c>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1">
+        <v>1</v>
+      </c>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="1"/>
+      <c r="P64" s="1">
+        <v>1</v>
+      </c>
+      <c r="S64">
+        <v>1</v>
+      </c>
+      <c r="W64">
+        <v>1</v>
+      </c>
+      <c r="Z64">
+        <v>1</v>
+      </c>
+      <c r="AD64">
+        <v>1</v>
+      </c>
+      <c r="AG64">
+        <v>1</v>
+      </c>
+      <c r="AK64">
+        <v>1</v>
+      </c>
+      <c r="AN64">
+        <v>1</v>
+      </c>
+      <c r="AW64">
+        <v>1</v>
+      </c>
+      <c r="BA64">
+        <v>1</v>
+      </c>
+      <c r="BF64">
+        <v>1</v>
+      </c>
+      <c r="BJ64">
+        <v>1</v>
+      </c>
+      <c r="BN64">
+        <v>1</v>
+      </c>
+      <c r="BP64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:68" x14ac:dyDescent="0.2">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1">
+        <v>1</v>
+      </c>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1">
+        <v>1</v>
+      </c>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1">
+        <v>1</v>
+      </c>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="1">
+        <v>1</v>
+      </c>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+      <c r="O65" s="1"/>
+      <c r="P65" s="1">
+        <v>1</v>
+      </c>
+      <c r="S65">
+        <v>1</v>
+      </c>
+      <c r="W65">
+        <v>1</v>
+      </c>
+      <c r="Z65">
+        <v>1</v>
+      </c>
+      <c r="AD65">
+        <v>1</v>
+      </c>
+      <c r="AG65">
+        <v>1</v>
+      </c>
+      <c r="AJ65">
+        <v>1</v>
+      </c>
+      <c r="AK65">
+        <v>1</v>
+      </c>
+      <c r="AN65">
+        <v>1</v>
+      </c>
+      <c r="AW65">
+        <v>1</v>
+      </c>
+      <c r="BA65">
+        <v>1</v>
+      </c>
+      <c r="BF65">
+        <v>1</v>
+      </c>
+      <c r="BI65">
+        <v>1</v>
+      </c>
+      <c r="BJ65">
+        <v>1</v>
+      </c>
+      <c r="BN65">
+        <v>1</v>
+      </c>
+      <c r="BP65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:68" x14ac:dyDescent="0.2">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1">
+        <v>1</v>
+      </c>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1">
+        <v>1</v>
+      </c>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1">
+        <v>1</v>
+      </c>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1">
+        <v>1</v>
+      </c>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="1"/>
+      <c r="P66" s="1">
+        <v>1</v>
+      </c>
+      <c r="T66">
+        <v>1</v>
+      </c>
+      <c r="U66">
+        <v>1</v>
+      </c>
+      <c r="V66">
+        <v>1</v>
+      </c>
+      <c r="Z66">
+        <v>1</v>
+      </c>
+      <c r="AA66">
+        <v>1</v>
+      </c>
+      <c r="AB66">
+        <v>1</v>
+      </c>
+      <c r="AC66">
+        <v>1</v>
+      </c>
+      <c r="AH66">
+        <v>1</v>
+      </c>
+      <c r="AI66">
+        <v>1</v>
+      </c>
+      <c r="AK66">
+        <v>1</v>
+      </c>
+      <c r="AN66">
+        <v>1</v>
+      </c>
+      <c r="AT66">
+        <v>1</v>
+      </c>
+      <c r="AU66">
+        <v>1</v>
+      </c>
+      <c r="AV66">
+        <v>1</v>
+      </c>
+      <c r="BB66">
+        <v>1</v>
+      </c>
+      <c r="BC66">
+        <v>1</v>
+      </c>
+      <c r="BG66">
+        <v>1</v>
+      </c>
+      <c r="BH66">
+        <v>1</v>
+      </c>
+      <c r="BJ66">
+        <v>1</v>
+      </c>
+      <c r="BO66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:68" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="1"/>
+      <c r="P67" s="1"/>
+      <c r="Z67">
+        <v>1</v>
+      </c>
+      <c r="AK67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:68" x14ac:dyDescent="0.2">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+      <c r="Z68">
+        <v>1</v>
+      </c>
+      <c r="AK68">
+        <v>1</v>
+      </c>
+      <c r="AL68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:68" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
+      <c r="O69" s="1"/>
+      <c r="P69" s="1"/>
+    </row>
+    <row r="70" spans="1:68" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
+      <c r="O70" s="1"/>
+      <c r="P70" s="1"/>
+    </row>
+    <row r="71" spans="1:68" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>11</v>
+      </c>
+      <c r="B71" t="s">
+        <v>60</v>
+      </c>
+      <c r="C71" t="s">
+        <v>60</v>
+      </c>
+      <c r="D71" t="s">
+        <v>60</v>
+      </c>
+      <c r="E71" t="s">
+        <v>60</v>
+      </c>
+      <c r="F71" t="s">
+        <v>60</v>
+      </c>
+      <c r="G71" t="s">
+        <v>60</v>
+      </c>
+      <c r="H71" t="s">
+        <v>60</v>
+      </c>
+      <c r="I71" t="s">
+        <v>60</v>
+      </c>
+      <c r="J71" t="s">
+        <v>60</v>
+      </c>
+      <c r="K71" t="s">
+        <v>61</v>
+      </c>
+      <c r="L71" t="s">
+        <v>61</v>
+      </c>
+      <c r="M71" t="s">
+        <v>61</v>
+      </c>
+      <c r="N71" t="s">
+        <v>61</v>
+      </c>
+      <c r="O71" t="s">
+        <v>61</v>
+      </c>
+      <c r="P71" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>61</v>
+      </c>
+      <c r="R71" t="s">
+        <v>62</v>
+      </c>
+      <c r="S71" t="s">
+        <v>62</v>
+      </c>
+      <c r="T71" t="s">
+        <v>62</v>
+      </c>
+      <c r="U71" t="s">
+        <v>62</v>
+      </c>
+      <c r="V71" t="s">
+        <v>62</v>
+      </c>
+      <c r="W71" t="s">
+        <v>62</v>
+      </c>
+      <c r="X71" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y71" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z71" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA71" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB71" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC71" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD71" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE71" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="72" spans="1:68" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+    </row>
+    <row r="73" spans="1:68" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+    </row>
+    <row r="74" spans="1:68" x14ac:dyDescent="0.2">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+    </row>
+    <row r="75" spans="1:68" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1">
+        <v>1</v>
+      </c>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="I75">
+        <v>1</v>
+      </c>
+      <c r="L75">
+        <v>1</v>
+      </c>
+      <c r="P75">
+        <v>1</v>
+      </c>
+      <c r="S75">
+        <v>1</v>
+      </c>
+      <c r="W75">
+        <v>1</v>
+      </c>
+      <c r="Z75">
+        <v>1</v>
+      </c>
+      <c r="AA75">
+        <v>1</v>
+      </c>
+      <c r="AB75">
+        <v>1</v>
+      </c>
+      <c r="AC75">
+        <v>1</v>
+      </c>
+      <c r="AD75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:68" x14ac:dyDescent="0.2">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1">
+        <v>1</v>
+      </c>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="I76">
+        <v>1</v>
+      </c>
+      <c r="M76">
+        <v>1</v>
+      </c>
+      <c r="O76">
+        <v>1</v>
+      </c>
+      <c r="S76">
+        <v>1</v>
+      </c>
+      <c r="W76">
+        <v>1</v>
+      </c>
+      <c r="AC76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:68" x14ac:dyDescent="0.2">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1">
+        <v>1</v>
+      </c>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="I77">
+        <v>1</v>
+      </c>
+      <c r="N77">
+        <v>1</v>
+      </c>
+      <c r="T77">
+        <v>1</v>
+      </c>
+      <c r="V77">
+        <v>1</v>
+      </c>
+      <c r="AB77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:68" x14ac:dyDescent="0.2">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1">
+        <v>1</v>
+      </c>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1">
+        <v>1</v>
+      </c>
+      <c r="H78">
+        <v>1</v>
+      </c>
+      <c r="M78">
+        <v>1</v>
+      </c>
+      <c r="O78">
+        <v>1</v>
+      </c>
+      <c r="T78">
+        <v>1</v>
+      </c>
+      <c r="V78">
+        <v>1</v>
+      </c>
+      <c r="AA78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:68" x14ac:dyDescent="0.2">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1">
+        <v>1</v>
+      </c>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1">
+        <v>1</v>
+      </c>
+      <c r="H79">
+        <v>1</v>
+      </c>
+      <c r="L79">
+        <v>1</v>
+      </c>
+      <c r="P79">
+        <v>1</v>
+      </c>
+      <c r="U79">
+        <v>1</v>
+      </c>
+      <c r="Z79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:68" x14ac:dyDescent="0.2">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1">
+        <v>1</v>
+      </c>
+      <c r="F80" s="1"/>
+      <c r="G80">
+        <v>1</v>
+      </c>
+      <c r="L80">
+        <v>1</v>
+      </c>
+      <c r="P80">
+        <v>1</v>
+      </c>
+      <c r="U80">
+        <v>1</v>
+      </c>
+      <c r="Z80">
+        <v>1</v>
+      </c>
+      <c r="AA80">
+        <v>1</v>
+      </c>
+      <c r="AB80">
+        <v>1</v>
+      </c>
+      <c r="AC80">
+        <v>1</v>
+      </c>
+      <c r="AD80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="U81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="S82">
+        <v>1</v>
+      </c>
+      <c r="T82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+    </row>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A29:A34 V29:XFD34 A3:XFD14 A17:XFD28">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+  <conditionalFormatting sqref="A43:A48 V43:XFD48 A3:XFD14 A17:XFD42">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B45:U53">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31:U39">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD1048576">
+  <conditionalFormatting sqref="A57:A62">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B59:P67">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A71:A76">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B73:F81">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>